<commit_message>
Putting things into functions and added an input
</commit_message>
<xml_diff>
--- a/Inbox/Dummy_FILE_A.xlsx
+++ b/Inbox/Dummy_FILE_A.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Python\Catalog Updater\Inbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241BDE9C-51F7-42ED-8FD3-F7C48B8D2FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A78D77-3F5F-4D8A-9DF4-5EEE141741A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{6A84965A-1668-4882-9922-9410E68867C3}"/>
+    <workbookView xWindow="10635" yWindow="2790" windowWidth="15855" windowHeight="11385" xr2:uid="{6A84965A-1668-4882-9922-9410E68867C3}"/>
   </bookViews>
   <sheets>
     <sheet name="File A" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'File A'!$A$2:$AT$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'File A'!$A$2:$AT$10</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -815,13 +815,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A4AA2F-9232-4CD7-AC80-DD3A6B036AB3}">
-  <dimension ref="A1:AT12"/>
+  <dimension ref="A1:AT10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="3" width="17.42578125" customWidth="1"/>
@@ -1002,7 +1000,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" ht="15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>22356568</v>
       </c>
@@ -1091,7 +1089,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" ht="15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>34256354</v>
       </c>
@@ -1198,7 +1196,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" ht="15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>44637355</v>
       </c>
@@ -1287,7 +1285,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" ht="15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>55261434</v>
       </c>
@@ -1394,7 +1392,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" ht="15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>66464788</v>
       </c>
@@ -1486,7 +1484,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" ht="15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>77423423</v>
       </c>
@@ -1575,7 +1573,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" ht="15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>88888856</v>
       </c>
@@ -1685,7 +1683,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" ht="15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>94757647</v>
       </c>
@@ -1792,7 +1790,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10342423</v>
       </c>
@@ -1893,11 +1891,6 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P11"/>
-      <c r="Q11"/>
-    </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding colors and fixing Data sheet importing
</commit_message>
<xml_diff>
--- a/Inbox/Dummy_FILE_A.xlsx
+++ b/Inbox/Dummy_FILE_A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Python\Catalog Updater\Inbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A78D77-3F5F-4D8A-9DF4-5EEE141741A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9074D5FB-FAF9-45DB-8438-7C2C09C488A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10635" yWindow="2790" windowWidth="15855" windowHeight="11385" xr2:uid="{6A84965A-1668-4882-9922-9410E68867C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A84965A-1668-4882-9922-9410E68867C3}"/>
   </bookViews>
   <sheets>
     <sheet name="File A" sheetId="1" r:id="rId1"/>
@@ -817,7 +817,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A4AA2F-9232-4CD7-AC80-DD3A6B036AB3}">
   <dimension ref="A1:AT10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1002,7 +1004,7 @@
     </row>
     <row r="2" spans="1:46" ht="15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>22356568</v>
+        <v>11111111</v>
       </c>
       <c r="B2" t="s">
         <v>67</v>
@@ -1047,10 +1049,10 @@
         <v>1</v>
       </c>
       <c r="P2" s="7">
-        <v>112.17</v>
+        <v>111.11</v>
       </c>
       <c r="Q2" s="7">
-        <v>7.3</v>
+        <v>100</v>
       </c>
       <c r="R2" t="s">
         <v>99</v>
@@ -1091,7 +1093,7 @@
     </row>
     <row r="3" spans="1:46" ht="15" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>34256354</v>
+        <v>24256354</v>
       </c>
       <c r="B3" t="s">
         <v>67</v>

</xml_diff>